<commit_message>
estructura historias de usuario
</commit_message>
<xml_diff>
--- a/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
+++ b/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MI PC\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A25B1E4-123D-4B29-BDE5-91DB8619D2DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -111,9 +112,6 @@
     <t>Cuando el cliente haga clic en una bicicleta específica para ver sus detalles.</t>
   </si>
   <si>
-    <t>La página mostrará todos los detalles de la bicicleta, incluyendo marca, modelo, tipo, descripción, precio, ofertas y opciones para agregar al carrito de compras.</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -180,9 +178,6 @@
     <t>Cuando el cliente quiera ver las reseñas y opiniones de otros compradores.</t>
   </si>
   <si>
-    <t>Se mostrarán las reseñas y opiniones de clientes anteriores en orden cronológico junto con las calificaciones y comentarios correspondientes</t>
-  </si>
-  <si>
     <t>6. Recuperar mi contraseña</t>
   </si>
   <si>
@@ -226,13 +221,30 @@
   </si>
   <si>
     <t>5.Crear una cuenta de usuario</t>
+  </si>
+  <si>
+    <r>
+      <t>La página mostrará todos los detalles de la bicicleta, incluyendo marca, modelo, tipo, descripción, precio, ofertas,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>stock y en caso de que el stock este en cero, una etiqueta de informe</t>
+    </r>
+  </si>
+  <si>
+    <t>Se mostrarán el promedio de las reseñas y opiniones de clientes anteriores en orden cronológico junto con las calificaciones y comentarios correspondientes, las reseñas y comentarios se limpiara cada cierto tiempo delimitado por el modelo de negocio ( 1 mes por ejemplo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +294,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -298,7 +316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,14 +359,17 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -357,9 +378,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -641,229 +659,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:8" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="7" t="s">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="7" t="s">
+    <row r="8" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualización del historias de usuario
</commit_message>
<xml_diff>
--- a/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
+++ b/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A25B1E4-123D-4B29-BDE5-91DB8619D2DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDDE5D5-0D0C-4A56-8998-8DBD814C05D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Historias de usuario y criterios de aceptación para un software que controla la calidad en la fabricación de repuestos para motos</t>
   </si>
@@ -112,12 +112,6 @@
     <t>Cuando el cliente haga clic en una bicicleta específica para ver sus detalles.</t>
   </si>
   <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
     <t>La lista de bicicletas se actualizará automáticamente para mostrar solo las bicicletas de la categoría seleccionada.</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
   </si>
   <si>
     <t>El cliente recibirá un enlace de restablecimiento por correo electrónico y podrá crear una nueva contraseña segura para su cuenta.</t>
-  </si>
-  <si>
-    <t>Baja</t>
   </si>
   <si>
     <t>5.Crear una cuenta de usuario</t>
@@ -238,6 +229,69 @@
   </si>
   <si>
     <t>Se mostrarán el promedio de las reseñas y opiniones de clientes anteriores en orden cronológico junto con las calificaciones y comentarios correspondientes, las reseñas y comentarios se limpiara cada cierto tiempo delimitado por el modelo de negocio ( 1 mes por ejemplo)</t>
+  </si>
+  <si>
+    <t>7. Buscador</t>
+  </si>
+  <si>
+    <t>Cliente quiero buscar un producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poder tener una barra de navegacion para buscar un producto especifico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar un producto en especifico que quiero ver </t>
+  </si>
+  <si>
+    <t>Que el cliente este en la pagina principla para poder buscar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando el cliente escriba y le de buscar, se muestre el resultado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cliente recibira su respuesta de la busqueda que hizo </t>
+  </si>
+  <si>
+    <t>8. Perfil de usuario</t>
+  </si>
+  <si>
+    <t>Poder visualizar mi informacion y poder modificar mis datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cliente se le guardara los cambio echos </t>
+  </si>
+  <si>
+    <t>Cuando el usuario modifique sus datos pueda guardar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el cliente este en el apartado de configuración </t>
+  </si>
+  <si>
+    <t>Cliente quiero poder visualizar y modificar mi perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poder visualizar y modificar mi informacion </t>
+  </si>
+  <si>
+    <t>9. Pedidos y compras</t>
+  </si>
+  <si>
+    <t>Cliente quiero visualizar mis pedidos, compras y poder modificar una compra</t>
+  </si>
+  <si>
+    <t>Poder visualizar mis compras y pedidos y modificar mi compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el cliente tiene que ingresar a los pedidos para poder visualizar y para ver y modificar las compras tiene que entrar al carrito y poder eliminar la compra o aunmentar el producto o disminuir la cantidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando modifique la compra se pueda visualizar tambien el cambio en el precio </t>
+  </si>
+  <si>
+    <t>Poder visualizar mis pedidos y  poder ver las compras en el carrito de compras</t>
+  </si>
+  <si>
+    <t>El cliente podra ver sus pedidos y modificar la cantidad de sus compras</t>
   </si>
 </sst>
 </file>
@@ -316,12 +370,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -353,11 +407,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -373,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -660,12 +728,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,140 +818,218 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>18</v>
+      <c r="H5" s="7">
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
+      <c r="H6" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizando las historias de usuario
</commit_message>
<xml_diff>
--- a/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
+++ b/documentacion/documentacion/estructuraHistoriaDeUsuario_bikestore_grupo_Coffe.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MI PC\OneDrive\Escritorio\BikeStore-Documentacion\documentacion\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDDE5D5-0D0C-4A56-8998-8DBD814C05D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Historias de usuario y criterios de aceptación para un software que controla la calidad en la fabricación de repuestos para motos</t>
   </si>
@@ -276,9 +275,6 @@
     <t>9. Pedidos y compras</t>
   </si>
   <si>
-    <t>Cliente quiero visualizar mis pedidos, compras y poder modificar una compra</t>
-  </si>
-  <si>
     <t>Poder visualizar mis compras y pedidos y modificar mi compra</t>
   </si>
   <si>
@@ -292,13 +288,43 @@
   </si>
   <si>
     <t>El cliente podra ver sus pedidos y modificar la cantidad de sus compras</t>
+  </si>
+  <si>
+    <t>Administrador interesado 
+en gestionar el inventario</t>
+  </si>
+  <si>
+    <t>Poder registrar nuevos
+productos</t>
+  </si>
+  <si>
+    <t>poder completar/actualizar el
+inventario del negocio</t>
+  </si>
+  <si>
+    <t>10.Registrar
+producto</t>
+  </si>
+  <si>
+    <t>que el administrador se encuentre en la pagina de registro de nuevo producto</t>
+  </si>
+  <si>
+    <t>cuando ingrese imagenes y 
+la informacion del nuevo producto</t>
+  </si>
+  <si>
+    <t>el administrador pueda recibir respuesta 
+de registro exitoso</t>
+  </si>
+  <si>
+    <t>Cliente quiero visualizar mis pedidos, compras y poder modificar una compra en el carrito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,8 +380,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +404,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -433,12 +472,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -446,6 +479,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,57 +775,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -798,7 +846,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="73.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="68.400000000000006" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -824,33 +872,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:8" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -869,40 +917,40 @@
       <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" ht="102.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="11">
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -928,109 +976,138 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:8" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:8" ht="102.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="6">
-        <v>2</v>
-      </c>
+      <c r="C13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>